<commit_message>
[#24] Organize pins spreadsheet. Create EncoderTest which updates encoder count. Attempt to put encoder interrupt into class currently unsuccessful.
</commit_message>
<xml_diff>
--- a/robot/rover/ArmDriverUnit/pins.xlsx
+++ b/robot/rover/ArmDriverUnit/pins.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vashm\Downloads\ArmDriverUnit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vashm\Documents\Git_Projects\robotics-prototype\robot\rover\ArmDriverUnit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0993D15-0A65-4BC6-BDF1-3C6B90B46741}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8327106F-EF3A-4A2A-924E-9D5E6F5E75F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{8E7351B4-E8C6-4347-8533-D0288101FE6D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{8E7351B4-E8C6-4347-8533-D0288101FE6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="33">
   <si>
     <t>pwm</t>
   </si>
@@ -121,6 +122,9 @@
   </si>
   <si>
     <t>T6</t>
+  </si>
+  <si>
+    <t>bit</t>
   </si>
 </sst>
 </file>
@@ -502,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75838143-F356-4457-BAE5-1C90F367D7C0}">
   <dimension ref="A3:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,169 +557,175 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
+      <c r="A8" s="2">
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>4</v>
+      <c r="A9" s="2">
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H9">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>5</v>
+      <c r="A10" s="2">
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
+      <c r="E10" t="s">
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
+      <c r="A12" s="2">
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>8</v>
+      <c r="A13" s="2">
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -723,169 +733,166 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>11</v>
+      <c r="A16" s="2">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H16">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H17">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>13</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
+      <c r="A19">
+        <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
+      <c r="A22" s="3">
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
+      <c r="A23">
+        <v>50</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
       <c r="G23" t="s">
         <v>9</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
+      <c r="A24" s="1">
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
@@ -893,49 +900,40 @@
         <v>10</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>21</v>
+      <c r="A26" s="1">
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G26" t="s">
         <v>10</v>
       </c>
       <c r="H26">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
+      <c r="A27" s="1">
+        <v>12</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>23</v>
+      <c r="A28" s="4">
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -947,401 +945,413 @@
         <v>12</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>24</v>
+      <c r="A29">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H29">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>25</v>
+      <c r="A30" s="4">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>26</v>
+      <c r="A31">
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H32">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>28</v>
+      <c r="A33" s="4">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H33">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
+      <c r="A34">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H34">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
         <v>5</v>
       </c>
       <c r="G35" t="s">
         <v>9</v>
       </c>
       <c r="H35">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
+      <c r="A36" s="4">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
       </c>
       <c r="E36" t="s">
         <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H36">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" t="s">
-        <v>5</v>
+      <c r="A37">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>33</v>
-      </c>
-      <c r="C38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
+      <c r="A38">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
       </c>
       <c r="H38">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>34</v>
+      <c r="A39" s="1">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
         <v>5</v>
       </c>
       <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41">
         <v>13</v>
       </c>
-      <c r="H39">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>35</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>36</v>
-      </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" t="s">
-        <v>5</v>
-      </c>
-      <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41">
-        <v>9</v>
-      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>37</v>
-      </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>5</v>
+      <c r="A42">
+        <v>52</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H42">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>38</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
+      <c r="A43" s="3">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="E43" t="s">
-        <v>5</v>
-      </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H43">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>39</v>
-      </c>
-      <c r="E44" t="s">
-        <v>5</v>
+      <c r="A44">
+        <v>51</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H44">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>40</v>
-      </c>
-      <c r="F45" t="s">
-        <v>7</v>
+      <c r="A45" s="3">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
       </c>
       <c r="G45" t="s">
         <v>11</v>
       </c>
       <c r="H45">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F46" t="s">
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>28</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>39</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>42</v>
-      </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>43</v>
-      </c>
-      <c r="F48" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>44</v>
-      </c>
-      <c r="F49" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>45</v>
-      </c>
-      <c r="F50" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>46</v>
-      </c>
-      <c r="F51" t="s">
-        <v>7</v>
+      <c r="B51" t="s">
+        <v>5</v>
       </c>
       <c r="G51" t="s">
         <v>9</v>
       </c>
       <c r="H51">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>47</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="A52" s="3">
         <v>30</v>
       </c>
-      <c r="D52" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" t="s">
-        <v>7</v>
+      <c r="B52" t="s">
+        <v>5</v>
       </c>
       <c r="G52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>48</v>
-      </c>
-      <c r="C53" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F53" t="s">
         <v>7</v>
       </c>
       <c r="G53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H53">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>49</v>
-      </c>
-      <c r="E54" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="F54" t="s">
         <v>7</v>
@@ -1350,15 +1360,12 @@
         <v>9</v>
       </c>
       <c r="H54">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>50</v>
-      </c>
-      <c r="E55" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F55" t="s">
         <v>7</v>
@@ -1367,115 +1374,752 @@
         <v>9</v>
       </c>
       <c r="H55">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F56" t="s">
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H56">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>52</v>
-      </c>
-      <c r="F57" t="s">
-        <v>7</v>
+      <c r="A57" s="4">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
       </c>
       <c r="G57" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H57">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>34</v>
+      </c>
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>53</v>
-      </c>
-      <c r="F58" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" t="s">
-        <v>10</v>
-      </c>
       <c r="H58">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>54</v>
-      </c>
-      <c r="F59" t="s">
-        <v>7</v>
+      <c r="A59" s="3">
+        <v>24</v>
       </c>
       <c r="G59" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H59">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H60">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F61" t="s">
         <v>7</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H61">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>57</v>
-      </c>
-      <c r="D62" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
       <c r="G62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H62">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A5:H62">
+    <sortCondition ref="H3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722535F0-9FA6-4856-BA24-8D834E546956}">
+  <dimension ref="A4:T20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.28515625" customWidth="1"/>
+    <col min="14" max="14" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5703125" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>56</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>57</v>
+      </c>
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>7</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="R7" s="4">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="N8" s="1">
+        <v>8</v>
+      </c>
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="R8" s="4">
+        <v>34</v>
+      </c>
+      <c r="S8" t="s">
+        <v>13</v>
+      </c>
+      <c r="T8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="N9" s="1">
+        <v>6</v>
+      </c>
+      <c r="O9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="R9" s="3">
+        <v>24</v>
+      </c>
+      <c r="S9" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>20</v>
+      </c>
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1">
+        <v>11</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="N11" s="2">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5</v>
+      </c>
+      <c r="O12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>16</v>
+      </c>
+      <c r="J13" s="4">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <v>47</v>
+      </c>
+      <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>17</v>
+      </c>
+      <c r="J14" s="4">
+        <v>36</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <v>48</v>
+      </c>
+      <c r="O14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F15" s="3">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="J15" s="4">
+        <v>37</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>55</v>
+      </c>
+      <c r="O15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4">
+        <v>38</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="N16">
+        <v>53</v>
+      </c>
+      <c r="O16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <v>52</v>
+      </c>
+      <c r="O17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>21</v>
+      </c>
+      <c r="N18">
+        <v>51</v>
+      </c>
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19">
+        <v>22</v>
+      </c>
+      <c r="N19">
+        <v>54</v>
+      </c>
+      <c r="O19" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>